<commit_message>
feat: add rpg data
</commit_message>
<xml_diff>
--- a/gameconf/rpg/enum.xlsx
+++ b/gameconf/rpg/enum.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>E|BUF类型-无|BuffEffectType|None|0</t>
   </si>
@@ -54,6 +54,12 @@
     <t>E|加权类型-无|BonusType|None|0</t>
   </si>
   <si>
+    <t>E|骰子-无|DiceType|None|0</t>
+  </si>
+  <si>
+    <t>E|媒介-无|DiceRule|None|0</t>
+  </si>
+  <si>
     <t>E|BUF类型-属性修改|BuffEffectType|STAT_MODIFIER|1</t>
   </si>
   <si>
@@ -78,6 +84,12 @@
     <t>E|加权类型-血量|BonusType|HP|1</t>
   </si>
   <si>
+    <t>E|骰子-点数1|DiceType|One|1</t>
+  </si>
+  <si>
+    <t>E|媒介-必选|DiceRule|Must|1</t>
+  </si>
+  <si>
     <t>E|BUF类型-状态附加|BuffEffectType|STATUS_EFFECT|2</t>
   </si>
   <si>
@@ -102,6 +114,12 @@
     <t>E|加权类型-内力|BonusType|MP|2</t>
   </si>
   <si>
+    <t>E|骰子-点数2|DiceType|Two|2</t>
+  </si>
+  <si>
+    <t>E|媒介-可选|DiceRule|Option|2</t>
+  </si>
+  <si>
     <t>E|BUF类型-持续伤害|BuffEffectType|DOT|3</t>
   </si>
   <si>
@@ -120,6 +138,12 @@
     <t>E|加权类型-基础攻击|BonusType|Attack|3</t>
   </si>
   <si>
+    <t>E|骰子-点数3|DiceType|Three|3</t>
+  </si>
+  <si>
+    <t>E|媒介-强化|DiceRule|Better|3</t>
+  </si>
+  <si>
     <t>E|BUF类型-持续治疗|BuffEffectType|HOT|4</t>
   </si>
   <si>
@@ -132,6 +156,9 @@
     <t>E|加权类型-基础防御|BonusType|Defense|4</t>
   </si>
   <si>
+    <t>E|骰子-点数4|DiceType|Four|4</t>
+  </si>
+  <si>
     <t>E|指向类型-所有盟友|TargetType|ALL_ALLIES|5</t>
   </si>
   <si>
@@ -141,6 +168,9 @@
     <t>E|加权类型-速度|BonusType|Speed|5</t>
   </si>
   <si>
+    <t>E|骰子-点数5|DiceType|Five|5</t>
+  </si>
+  <si>
     <t>E|指向类型-不分敌我|TargetType|ALL|6</t>
   </si>
   <si>
@@ -150,19 +180,34 @@
     <t>E|加权类型-等级|BonusType|Level|6</t>
   </si>
   <si>
+    <t>E|骰子-点数6|DiceType|Six|6</t>
+  </si>
+  <si>
     <t>E|触发条件-回合开始|TriggerType|TURNBEFORE|7</t>
   </si>
   <si>
     <t>E|加权类型-力量|BonusType|Strength|7</t>
   </si>
   <si>
+    <t>E|骰子-奇数|DiceType|Odd|7</t>
+  </si>
+  <si>
     <t>E|触发条件-回合结束|TriggerType|TURNAFTER|8</t>
   </si>
   <si>
     <t>E|加权类型-灵敏|BonusType|Agility|8</t>
   </si>
   <si>
+    <t>E|骰子-偶数|DiceType|Even|8</t>
+  </si>
+  <si>
+    <t>E|触发条件-持续生效|TriggerType|HOLD|9</t>
+  </si>
+  <si>
     <t>E|加权类型-悟性|BonusType|Intelligence|9</t>
+  </si>
+  <si>
+    <t>E|骰子-任意|DiceType|All|9</t>
   </si>
   <si>
     <t>E|加权类型-根骨|BonusType|Vitality|10</t>
@@ -1108,13 +1153,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="27.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
@@ -1123,10 +1168,12 @@
     <col min="5" max="5" width="33.375" customWidth="1"/>
     <col min="6" max="6" width="31.125" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="31.125" customWidth="1"/>
+    <col min="8" max="8" width="21.125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1151,154 +1198,199 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="6" spans="6:8">
+    <row r="6" spans="6:9">
       <c r="F6" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="7" spans="6:8">
+    <row r="7" spans="6:9">
       <c r="F7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="7:8">
+    <row r="8" spans="7:9">
       <c r="G8" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="9" spans="7:8">
+    <row r="9" spans="7:9">
       <c r="G9" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="10" spans="8:8">
+    <row r="10" spans="7:9">
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>58</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="8:8">
       <c r="H11" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="8:8">
       <c r="H12" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="8:8">
       <c r="H13" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="8:8">
       <c r="H14" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1324,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: change framework route manger
</commit_message>
<xml_diff>
--- a/gameconf/rpg/enum.xlsx
+++ b/gameconf/rpg/enum.xlsx
@@ -1153,243 +1153,243 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="27.5" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="22.75" customWidth="1"/>
-    <col min="4" max="4" width="21.375" customWidth="1"/>
-    <col min="5" max="5" width="33.375" customWidth="1"/>
-    <col min="6" max="6" width="31.125" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="2" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="33.375" customWidth="1"/>
+    <col min="7" max="7" width="31.125" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+    <col min="9" max="9" width="21.125" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>39</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>40</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="6:9">
-      <c r="F6" t="s">
+    <row r="6" spans="7:10">
+      <c r="G6" t="s">
         <v>43</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>44</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>45</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="6:9">
-      <c r="F7" t="s">
+    <row r="7" spans="7:10">
+      <c r="G7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="7:9">
-      <c r="G8" t="s">
+    <row r="8" spans="8:10">
+      <c r="H8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="7:9">
-      <c r="G9" t="s">
+    <row r="9" spans="8:10">
+      <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>55</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="7:9">
-      <c r="G10" t="s">
+    <row r="10" spans="8:10">
+      <c r="H10" t="s">
         <v>57</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>58</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="8:8">
-      <c r="H11" t="s">
+    <row r="11" spans="9:9">
+      <c r="I11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="8:8">
-      <c r="H12" t="s">
+    <row r="12" spans="9:9">
+      <c r="I12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="8:8">
-      <c r="H13" t="s">
+    <row r="13" spans="9:9">
+      <c r="I13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="8:8">
-      <c r="H14" t="s">
+    <row r="14" spans="9:9">
+      <c r="I14" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>